<commit_message>
Butoes para exportar os datatables
</commit_message>
<xml_diff>
--- a/logs/log_execution.xlsx
+++ b/logs/log_execution.xlsx
@@ -387,7 +387,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1661861225.04203</t>
+          <t>2022-08-30 17:08:31</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -414,7 +414,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1661861227.17855</t>
+          <t>2022-08-30 17:08:32</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -441,7 +441,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1661861228.76211</t>
+          <t>2022-08-30 17:08:33</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -456,7 +456,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD TX PVLS</t>
+          <t>Buscar valores para cada indicador: DSD TX NEW</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -468,7 +468,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1661861242.80523</t>
+          <t>2022-08-30 17:08:38</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD TB ART</t>
+          <t>Buscar valores para cada indicador: DSD TX CURR</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">

</xml_diff>

<commit_message>
Save upload info(dataframes, indicators, datwes) after sending to dhis
</commit_message>
<xml_diff>
--- a/logs/log_execution.xlsx
+++ b/logs/log_execution.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,17 +387,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-09-01 16:08:01</t>
+          <t>2022-09-06 13:43:03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MER_CT_1Maio_15</t>
+          <t>MER_ATS_Xipamanine_12</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MER C&amp;T</t>
+          <t>MER ATS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -414,17 +414,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2022-09-01 16:08:03</t>
+          <t>2022-09-06 13:43:04</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MER_CT_1Maio_15</t>
+          <t>MER_ATS_Xipamanine_12</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MER C&amp;T</t>
+          <t>MER ATS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -441,25 +441,106 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2022-09-01 16:08:05</t>
+          <t>2022-09-06 13:43:10</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MER_CT_1Maio_15</t>
+          <t>MER_ATS_Xipamanine_12</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MER C&amp;T</t>
+          <t>MER ATS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD TX NEW</t>
+          <t>Buscar valores para cada indicador: DSD HTS TST</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2022-09-06 13:44:00</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MER_ATS_Xipamanine_12</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MER ATS</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS INDEX</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2022-09-06 13:44:29</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MER_ATS_Xipamanine_12</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MER ATS</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS SELF</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2022-09-06 13:44:41</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MER_ATS_Xipamanine_12</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>MER ATS</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD TB STAT</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>ok</t>
         </is>

</xml_diff>

<commit_message>
bug  fixed for ct dataset
</commit_message>
<xml_diff>
--- a/logs/log_execution.xlsx
+++ b/logs/log_execution.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,17 +387,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-09-06 13:43:03</t>
+          <t>2022-09-06 22:53:48</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_12</t>
+          <t>MER_CT_Bagamoio_24</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MER ATS</t>
+          <t>MER C&amp;T</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -414,17 +414,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2022-09-06 13:43:04</t>
+          <t>2022-09-06 22:53:49</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_12</t>
+          <t>MER_CT_Bagamoio_24</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MER ATS</t>
+          <t>MER C&amp;T</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -441,22 +441,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2022-09-06 13:43:10</t>
+          <t>2022-09-06 22:53:49</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_12</t>
+          <t>MER_CT_Bagamoio_24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MER ATS</t>
+          <t>MER C&amp;T</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD HTS TST</t>
+          <t>Buscar valores para cada indicador: DSD TX NEW</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -468,22 +468,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2022-09-06 13:44:00</t>
+          <t>2022-09-06 22:53:52</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_12</t>
+          <t>MER_CT_Bagamoio_24</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MER ATS</t>
+          <t>MER C&amp;T</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD HTS INDEX</t>
+          <t>Buscar valores para cada indicador: DSD TX CURR</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -495,22 +495,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2022-09-06 13:44:29</t>
+          <t>2022-09-06 22:53:56</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_12</t>
+          <t>MER_CT_Bagamoio_24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MER ATS</t>
+          <t>MER C&amp;T</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD HTS SELF</t>
+          <t>Buscar valores para cada indicador: DSD TX RTT</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -522,25 +522,133 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2022-09-06 13:44:41</t>
+          <t>2022-09-06 22:54:01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_12</t>
+          <t>MER_CT_Bagamoio_24</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MER ATS</t>
+          <t>MER C&amp;T</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD TB STAT</t>
+          <t>Buscar valores para cada indicador: DSD TX ML</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2022-09-06 22:54:14</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MER_CT_Bagamoio_24</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD PMCT ART</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2022-09-06 22:54:15</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MER_CT_Bagamoio_24</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD TX PVLS</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2022-09-06 22:54:21</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MER_CT_Bagamoio_24</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD TX TB</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2022-09-06 22:54:25</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MER_CT_Bagamoio_24</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MER C&amp;T</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD TB ART</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>ok</t>
         </is>

</xml_diff>

<commit_message>
Minor Bug fixlserver funtion
</commit_message>
<xml_diff>
--- a/logs/log_execution.xlsx
+++ b/logs/log_execution.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,12 +387,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-09-13 22:50:57</t>
+          <t>2022-09-14 22:23:42</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -414,12 +414,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2022-09-13 22:50:58</t>
+          <t>2022-09-14 22:23:43</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -441,12 +441,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2022-09-13 22:50:59</t>
+          <t>2022-09-14 22:23:45</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -468,12 +468,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2022-09-13 22:51:03</t>
+          <t>2022-09-14 22:23:53</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -495,12 +495,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2022-09-13 22:51:09</t>
+          <t>2022-09-14 22:24:04</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -522,12 +522,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2022-09-13 22:51:20</t>
+          <t>2022-09-14 22:24:18</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -549,12 +549,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2022-09-13 22:52:06</t>
+          <t>2022-09-14 22:24:53</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -576,12 +576,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2022-09-13 22:52:21</t>
+          <t>2022-09-14 22:24:56</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -603,12 +603,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2022-09-13 22:53:08</t>
+          <t>2022-09-14 22:25:12</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MER_CT_Romao_14</t>
+          <t>MER_CT_ChamanculoCS_37</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -622,33 +622,6 @@
         </is>
       </c>
       <c r="E11" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2022-09-13 22:53:14</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MER_CT_Romao_14</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>MER C&amp;T</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Buscar valores para cada indicador: DSD TB ART</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
         <is>
           <t>ok</t>
         </is>

</xml_diff>

<commit_message>
store log files on Gdrive
</commit_message>
<xml_diff>
--- a/logs/log_execution.xlsx
+++ b/logs/log_execution.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,17 +387,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-09-14 22:23:42</t>
+          <t>2022-09-20 13:35:17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MER_CT_ChamanculoCS_37</t>
+          <t>MER_SMI_1Junho_8</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MER C&amp;T</t>
+          <t>MER SMI</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -414,17 +414,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2022-09-14 22:23:43</t>
+          <t>2022-09-20 13:35:18</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MER_CT_ChamanculoCS_37</t>
+          <t>MER_SMI_1Junho_8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MER C&amp;T</t>
+          <t>MER SMI</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -441,22 +441,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2022-09-14 22:23:45</t>
+          <t>2022-09-20 13:35:18</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MER_CT_ChamanculoCS_37</t>
+          <t>MER_SMI_1Junho_8</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MER C&amp;T</t>
+          <t>MER SMI</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD TX NEW</t>
+          <t>Buscar valores para cada indicador: DSD PMTCT EID</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -468,160 +468,25 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2022-09-14 22:23:53</t>
+          <t>2022-09-20 13:35:19</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MER_CT_ChamanculoCS_37</t>
+          <t>MER_SMI_1Junho_8</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MER C&amp;T</t>
+          <t>MER SMI</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD TX CURR</t>
+          <t>Buscar valores para cada indicador: DSD PMTCT HEI POS</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2022-09-14 22:24:04</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>MER_CT_ChamanculoCS_37</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>MER C&amp;T</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Buscar valores para cada indicador: DSD TX RTT</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2022-09-14 22:24:18</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>MER_CT_ChamanculoCS_37</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>MER C&amp;T</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Buscar valores para cada indicador: DSD TX ML</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2022-09-14 22:24:53</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>MER_CT_ChamanculoCS_37</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>MER C&amp;T</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Buscar valores para cada indicador: DSD PMCT ART</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2022-09-14 22:24:56</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>MER_CT_ChamanculoCS_37</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>MER C&amp;T</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Buscar valores para cada indicador: DSD TX PVLS</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2022-09-14 22:25:12</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>MER_CT_ChamanculoCS_37</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>MER C&amp;T</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Buscar valores para cada indicador: DSD TX TB</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
         <is>
           <t>ok</t>
         </is>

</xml_diff>

<commit_message>
Bug fix: problem woht excell upload history
</commit_message>
<xml_diff>
--- a/logs/log_execution.xlsx
+++ b/logs/log_execution.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,17 +387,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-01-16 14:16:52.72</t>
+          <t>2025-07-30 16:24:10.51</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_41</t>
+          <t>MER_ATSC_Kamavota_51</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MER PREVENTION</t>
+          <t>MER ATS COMMUNITY</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -414,17 +414,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-01-16 14:16:52.97</t>
+          <t>2025-07-30 16:24:10.68</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_41</t>
+          <t>MER_ATSC_Kamavota_51</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MER PREVENTION</t>
+          <t>MER ATS COMMUNITY</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -441,22 +441,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-01-16 14:16:53.03</t>
+          <t>2025-07-30 16:24:10.75</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_41</t>
+          <t>MER_ATSC_Kamavota_51</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MER PREVENTION</t>
+          <t>MER ATS COMMUNITY</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD PREP</t>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY OTHER</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -468,22 +468,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-01-16 14:16:55.79</t>
+          <t>2025-07-30 16:24:12.03</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_41</t>
+          <t>MER_ATSC_Kamavota_51</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MER PREVENTION</t>
+          <t>MER ATS COMMUNITY</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD TB PREV</t>
+          <t>Buscar valores para cada indicador: DSD HTS INDEX COMMUNITY</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -495,22 +495,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-01-16 14:16:56.90</t>
+          <t>2025-07-30 16:24:15.51</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_41</t>
+          <t>MER_ATSC_Kamavota_51</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MER PREVENTION</t>
+          <t>MER ATS COMMUNITY</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD GEND GBV</t>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY MOBILE</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -522,25 +522,808 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-01-16 14:16:59.18</t>
+          <t>2025-07-30 16:24:18.76</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MER_ATS_Xipamanine_41</t>
+          <t>MER_ATSC_Kamaxakeni_52</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MER PREVENTION</t>
+          <t>MER ATS COMMUNITY</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Buscar valores para cada indicador: DSD FPINT SITE</t>
+          <t>Verficar a integridade do ficheiro de importacao</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:18.90</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamaxakeni_52</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Verificar se todos os dataElements do Ficheiro de Mapeamento existem no DHIS2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:18.94</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamaxakeni_52</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY OTHER</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:20.36</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamaxakeni_52</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS INDEX COMMUNITY</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:23.79</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamaxakeni_52</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY MOBILE</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:27.06</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kampfumu_53</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Verficar a integridade do ficheiro de importacao</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:27.20</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kampfumu_53</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Verificar se todos os dataElements do Ficheiro de Mapeamento existem no DHIS2</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:27.23</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kampfumu_53</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY OTHER</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:28.74</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kampfumu_53</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS INDEX COMMUNITY</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:32.27</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kampfumu_53</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY MOBILE</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:35.46</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamubukwana_54</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Verficar a integridade do ficheiro de importacao</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:35.58</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamubukwana_54</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Verificar se todos os dataElements do Ficheiro de Mapeamento existem no DHIS2</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:35.62</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamubukwana_54</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY OTHER</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:36.91</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamubukwana_54</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS INDEX COMMUNITY</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:40.30</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kamubukwana_54</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY MOBILE</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:43.53</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Katembe_55</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Verficar a integridade do ficheiro de importacao</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:43.65</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Katembe_55</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Verificar se todos os dataElements do Ficheiro de Mapeamento existem no DHIS2</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:43.69</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Katembe_55</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY OTHER</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:44.97</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Katembe_55</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS INDEX COMMUNITY</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:48.56</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Katembe_55</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY MOBILE</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:51.74</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kanyaka_56</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Verficar a integridade do ficheiro de importacao</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:51.87</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kanyaka_56</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Verificar se todos os dataElements do Ficheiro de Mapeamento existem no DHIS2</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:51.90</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kanyaka_56</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY OTHER</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:53.15</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kanyaka_56</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS INDEX COMMUNITY</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:24:56.85</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Kanyaka_56</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY MOBILE</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:25:00.32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Nlhamankulu_57</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Verficar a integridade do ficheiro de importacao</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:25:00.45</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Nlhamankulu_57</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Verificar se todos os dataElements do Ficheiro de Mapeamento existem no DHIS2</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:25:00.49</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Nlhamankulu_57</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY OTHER</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>processando...</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:25:01.92</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Nlhamankulu_57</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS INDEX COMMUNITY</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-07-30 16:25:05.77</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>MER_ATSC_Nlhamankulu_57</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>MER ATS COMMUNITY</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Buscar valores para cada indicador: DSD HTS TST COMMUNITY MOBILE</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>ok</t>
         </is>

</xml_diff>